<commit_message>
Modified core files for an accurate data extraction
</commit_message>
<xml_diff>
--- a/Data Sets/Analysis Data/Stops Sorted Future Network.xlsx
+++ b/Data Sets/Analysis Data/Stops Sorted Future Network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sulemanbasit/PycharmProjects/Calgary-Transit-Economic-Gap-Analysis/Data Sets/Analysis Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B22059-BA37-EE4E-BBB6-5B98A6284C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D147368-74D5-4948-BE00-33F0FAD6959A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="12980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16700" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="608">
   <si>
     <t>Location</t>
   </si>
@@ -1860,9 +1860,6 @@
     <t>50.963583,-114.012232</t>
   </si>
   <si>
-    <t>douglas glen blvd</t>
-  </si>
-  <si>
     <t>50.957148,-114.007522</t>
   </si>
   <si>
@@ -1972,11 +1969,6 @@
   </si>
   <si>
     <t>50.936424,-114.117873</t>
-  </si>
-  <si>
-    <t>Shaganappi
-Rosscarrock
-Killarney</t>
   </si>
   <si>
     <t>Hounsfield Heights/Briar Hill</t>
@@ -1996,6 +1988,51 @@
 Glamorgan
 Glenbrook
 Killarney/Glengarry</t>
+  </si>
+  <si>
+    <t>Winston Heights/Mountview
+Renfrew</t>
+  </si>
+  <si>
+    <t>Downtown Commercial Core
+Downtown East Village</t>
+  </si>
+  <si>
+    <t>Downtown Commercial Core
+Beltline
+Downtown East Village</t>
+  </si>
+  <si>
+    <t>Downtown East Village
+Beltline</t>
+  </si>
+  <si>
+    <t>Downtown East Village
+Beltline
+Ramsay
+Inglewood</t>
+  </si>
+  <si>
+    <t>Douglasdale/Glen blvd</t>
+  </si>
+  <si>
+    <t>Crescent Heights
+Winston Heights/Mountview
+Tuxedo Park
+Renfrew</t>
+  </si>
+  <si>
+    <t>Shaganappi
+Rosscarrock
+Killarney/Glengarry</t>
+  </si>
+  <si>
+    <t>Ogden
+Riverbend</t>
+  </si>
+  <si>
+    <t>Ogden
+Douglasdale/Glen</t>
   </si>
 </sst>
 </file>
@@ -5903,11 +5940,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A64457-543D-5E4D-939D-9DB06646213E}">
   <dimension ref="A1:D220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="J102" sqref="J102"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -5923,7 +5965,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>211</v>
       </c>
@@ -5951,7 +5993,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>215</v>
       </c>
@@ -5965,7 +6007,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>217</v>
       </c>
@@ -6105,7 +6147,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
         <v>237</v>
       </c>
@@ -6119,7 +6161,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>239</v>
       </c>
@@ -6245,7 +6287,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>248</v>
       </c>
@@ -6259,7 +6301,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>250</v>
       </c>
@@ -6273,7 +6315,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
         <v>251</v>
       </c>
@@ -6287,7 +6329,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
         <v>252</v>
       </c>
@@ -6413,7 +6455,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
         <v>268</v>
       </c>
@@ -6441,7 +6483,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
         <v>272</v>
       </c>
@@ -6469,7 +6511,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
         <v>276</v>
       </c>
@@ -6581,7 +6623,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="23" t="s">
         <v>288</v>
       </c>
@@ -6665,7 +6707,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="24" t="s">
         <v>297</v>
       </c>
@@ -6735,7 +6777,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="25" t="s">
         <v>307</v>
       </c>
@@ -6749,7 +6791,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="25" t="s">
         <v>309</v>
       </c>
@@ -6763,7 +6805,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A62" s="25" t="s">
         <v>310</v>
       </c>
@@ -6777,7 +6819,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="25" t="s">
         <v>297</v>
       </c>
@@ -6981,7 +7023,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A78" s="33" t="s">
         <v>403</v>
       </c>
@@ -7009,7 +7051,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="33" t="s">
         <v>408</v>
       </c>
@@ -7023,7 +7065,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="33" t="s">
         <v>411</v>
       </c>
@@ -7037,7 +7079,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="33" t="s">
         <v>414</v>
       </c>
@@ -7051,7 +7093,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A83" s="33" t="s">
         <v>417</v>
       </c>
@@ -7065,7 +7107,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="33" t="s">
         <v>420</v>
       </c>
@@ -7079,7 +7121,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="33" t="s">
         <v>423</v>
       </c>
@@ -7244,12 +7286,12 @@
         <v>473</v>
       </c>
       <c r="D96" s="33" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="33" t="s">
-        <v>145</v>
+        <v>453</v>
       </c>
       <c r="B97" s="33" t="s">
         <v>452</v>
@@ -7275,7 +7317,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="33" t="s">
         <v>239</v>
       </c>
@@ -7289,7 +7331,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A100" s="33" t="s">
         <v>458</v>
       </c>
@@ -7345,7 +7387,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>51</v>
       </c>
@@ -7398,7 +7440,7 @@
         <v>52</v>
       </c>
       <c r="D107" s="26" t="s">
-        <v>595</v>
+        <v>605</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7429,7 +7471,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>63</v>
       </c>
@@ -7454,7 +7496,7 @@
         <v>52</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -7468,7 +7510,7 @@
         <v>52</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -7482,7 +7524,7 @@
         <v>52</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -7496,7 +7538,7 @@
         <v>52</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -7555,7 +7597,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>72</v>
       </c>
@@ -7650,7 +7692,7 @@
         <v>7</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -7664,7 +7706,7 @@
         <v>7</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -7678,7 +7720,7 @@
         <v>7</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -7692,7 +7734,7 @@
         <v>7</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7751,7 +7793,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>15</v>
       </c>
@@ -7790,7 +7832,7 @@
         <v>7</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -7863,7 +7905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>30</v>
       </c>
@@ -7919,7 +7961,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>38</v>
       </c>
@@ -7933,7 +7975,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>40</v>
       </c>
@@ -8003,7 +8045,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="16" t="s">
         <v>87</v>
       </c>
@@ -8031,7 +8073,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A153" s="16" t="s">
         <v>91</v>
       </c>
@@ -8042,7 +8084,7 @@
         <v>83</v>
       </c>
       <c r="D153" s="36" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8059,7 +8101,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A155" s="16" t="s">
         <v>95</v>
       </c>
@@ -8073,7 +8115,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A156" s="16" t="s">
         <v>97</v>
       </c>
@@ -8084,10 +8126,10 @@
         <v>83</v>
       </c>
       <c r="D156" s="36" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="16" t="s">
         <v>99</v>
       </c>
@@ -8098,10 +8140,10 @@
         <v>83</v>
       </c>
       <c r="D157" s="36" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="16" t="s">
         <v>100</v>
       </c>
@@ -8227,7 +8269,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
         <v>115</v>
       </c>
@@ -8238,10 +8280,10 @@
         <v>117</v>
       </c>
       <c r="D167" s="37" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A168" s="17" t="s">
         <v>535</v>
       </c>
@@ -8252,7 +8294,7 @@
         <v>117</v>
       </c>
       <c r="D168" s="37" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -8297,7 +8339,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="17" t="s">
         <v>125</v>
       </c>
@@ -8311,7 +8353,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
         <v>127</v>
       </c>
@@ -8325,7 +8367,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="17" t="s">
         <v>544</v>
       </c>
@@ -8339,7 +8381,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A175" s="17" t="s">
         <v>546</v>
       </c>
@@ -8420,35 +8462,35 @@
         <v>117</v>
       </c>
       <c r="D180" s="37" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="B181" s="17" t="s">
         <v>557</v>
-      </c>
-      <c r="B181" s="17" t="s">
-        <v>558</v>
       </c>
       <c r="C181" s="17" t="s">
         <v>117</v>
       </c>
       <c r="D181" s="37" t="s">
-        <v>143</v>
+        <v>607</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="B182" s="17" t="s">
         <v>559</v>
-      </c>
-      <c r="B182" s="17" t="s">
-        <v>560</v>
       </c>
       <c r="C182" s="17" t="s">
         <v>117</v>
       </c>
       <c r="D182" s="17" t="s">
-        <v>145</v>
+        <v>453</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
@@ -8456,7 +8498,7 @@
         <v>146</v>
       </c>
       <c r="B183" s="18" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C183" s="18" t="s">
         <v>148</v>
@@ -8470,7 +8512,7 @@
         <v>149</v>
       </c>
       <c r="B184" s="18" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C184" s="18" t="s">
         <v>148</v>
@@ -8479,26 +8521,26 @@
         <v>147</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="18" t="s">
         <v>150</v>
       </c>
       <c r="B185" s="18" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C185" s="18" t="s">
         <v>148</v>
       </c>
       <c r="D185" s="38" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A186" s="18" t="s">
         <v>152</v>
       </c>
       <c r="B186" s="18" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C186" s="18" t="s">
         <v>148</v>
@@ -8507,18 +8549,18 @@
         <v>153</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A187" s="18" t="s">
         <v>154</v>
       </c>
       <c r="B187" s="18" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C187" s="18" t="s">
         <v>148</v>
       </c>
       <c r="D187" s="38" t="s">
-        <v>155</v>
+        <v>600</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8526,13 +8568,13 @@
         <v>156</v>
       </c>
       <c r="B188" s="18" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C188" s="18" t="s">
         <v>148</v>
       </c>
       <c r="D188" s="38" t="s">
-        <v>157</v>
+        <v>601</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -8540,13 +8582,13 @@
         <v>158</v>
       </c>
       <c r="B189" s="18" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C189" s="18" t="s">
         <v>148</v>
       </c>
       <c r="D189" s="38" t="s">
-        <v>159</v>
+        <v>602</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8554,7 +8596,7 @@
         <v>160</v>
       </c>
       <c r="B190" s="18" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C190" s="18" t="s">
         <v>148</v>
@@ -8568,7 +8610,7 @@
         <v>162</v>
       </c>
       <c r="B191" s="18" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C191" s="18" t="s">
         <v>148</v>
@@ -8582,7 +8624,7 @@
         <v>164</v>
       </c>
       <c r="B192" s="18" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C192" s="18" t="s">
         <v>148</v>
@@ -8596,7 +8638,7 @@
         <v>166</v>
       </c>
       <c r="B193" s="18" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C193" s="18" t="s">
         <v>148</v>
@@ -8605,12 +8647,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A194" s="18" t="s">
         <v>167</v>
       </c>
       <c r="B194" s="18" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C194" s="18" t="s">
         <v>148</v>
@@ -8619,12 +8661,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B195" s="18" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C195" s="18" t="s">
         <v>148</v>
@@ -8633,12 +8675,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A196" s="18" t="s">
         <v>171</v>
       </c>
       <c r="B196" s="18" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C196" s="18" t="s">
         <v>148</v>
@@ -8647,12 +8689,12 @@
         <v>172</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="18" t="s">
         <v>173</v>
       </c>
       <c r="B197" s="18" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C197" s="18" t="s">
         <v>148</v>
@@ -8666,7 +8708,7 @@
         <v>175</v>
       </c>
       <c r="B198" s="18" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C198" s="18" t="s">
         <v>148</v>
@@ -8680,7 +8722,7 @@
         <v>177</v>
       </c>
       <c r="B199" s="18" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C199" s="18" t="s">
         <v>148</v>
@@ -8694,7 +8736,7 @@
         <v>178</v>
       </c>
       <c r="B200" s="18" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C200" s="18" t="s">
         <v>148</v>
@@ -8703,12 +8745,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="19" t="s">
         <v>179</v>
       </c>
       <c r="B201" s="19" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C201" s="19" t="s">
         <v>181</v>
@@ -8722,7 +8764,7 @@
         <v>182</v>
       </c>
       <c r="B202" s="19" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C202" s="19" t="s">
         <v>181</v>
@@ -8736,7 +8778,7 @@
         <v>183</v>
       </c>
       <c r="B203" s="19" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C203" s="19" t="s">
         <v>181</v>
@@ -8745,12 +8787,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A204" s="19" t="s">
         <v>184</v>
       </c>
       <c r="B204" s="19" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C204" s="19" t="s">
         <v>181</v>
@@ -8764,7 +8806,7 @@
         <v>186</v>
       </c>
       <c r="B205" s="19" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C205" s="19" t="s">
         <v>181</v>
@@ -8778,7 +8820,7 @@
         <v>187</v>
       </c>
       <c r="B206" s="19" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C206" s="19" t="s">
         <v>181</v>
@@ -8787,12 +8829,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A207" s="19" t="s">
         <v>188</v>
       </c>
       <c r="B207" s="19" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C207" s="19" t="s">
         <v>181</v>
@@ -8801,12 +8843,12 @@
         <v>189</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A208" s="19" t="s">
         <v>190</v>
       </c>
       <c r="B208" s="19" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C208" s="19" t="s">
         <v>181</v>
@@ -8820,7 +8862,7 @@
         <v>192</v>
       </c>
       <c r="B209" s="19" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C209" s="19" t="s">
         <v>181</v>
@@ -8829,12 +8871,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A210" s="19" t="s">
         <v>194</v>
       </c>
       <c r="B210" s="19" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C210" s="19" t="s">
         <v>181</v>
@@ -8857,7 +8899,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A212" s="19" t="s">
         <v>197</v>
       </c>
@@ -8871,7 +8913,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A213" s="19" t="s">
         <v>198</v>
       </c>
@@ -8885,7 +8927,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="19" t="s">
         <v>199</v>
       </c>
@@ -8904,7 +8946,7 @@
         <v>200</v>
       </c>
       <c r="B215" s="19" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C215" s="19" t="s">
         <v>181</v>
@@ -8918,7 +8960,7 @@
         <v>202</v>
       </c>
       <c r="B216" s="19" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C216" s="19" t="s">
         <v>181</v>
@@ -8932,7 +8974,7 @@
         <v>204</v>
       </c>
       <c r="B217" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C217" s="19" t="s">
         <v>181</v>
@@ -8946,7 +8988,7 @@
         <v>206</v>
       </c>
       <c r="B218" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C218" s="19" t="s">
         <v>181</v>
@@ -8960,7 +9002,7 @@
         <v>208</v>
       </c>
       <c r="B219" s="19" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C219" s="19" t="s">
         <v>181</v>
@@ -8974,7 +9016,7 @@
         <v>210</v>
       </c>
       <c r="B220" s="19" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C220" s="19" t="s">
         <v>181</v>

</xml_diff>